<commit_message>
Support columns of function types
</commit_message>
<xml_diff>
--- a/src/test-haxe/com/qifun/importCsv/TestConfig.xlsx
+++ b/src/test-haxe/com/qifun/importCsv/TestConfig.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Foo" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,13 @@
     <sheet name="import" sheetId="4" r:id="rId4"/>
     <sheet name="using" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <webPublishing codePage="65001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>"中文"</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,14 @@
   </si>
   <si>
     <t>com.qifun.importCsv.StringInterpolation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f:Void-&gt;String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function()return ""</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,13 +614,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -625,7 +633,7 @@
     <col min="6" max="6" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="41.25" thickBot="1">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="41.25" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -647,13 +655,16 @@
       <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1">
+      <c r="H1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
@@ -667,8 +678,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1"/>
-    <row r="5" spans="1:7">
+    <row r="4" spans="1:8" s="2" customFormat="1"/>
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -681,28 +692,31 @@
       <c r="G5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="7" customFormat="1">
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="7" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="135">
+    <row r="10" spans="1:8" ht="135">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -710,17 +724,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -854,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="A20:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>